<commit_message>
Address creation fixes and changes necessary for IRK api changes.
</commit_message>
<xml_diff>
--- a/src/main/webapp/src/assets/files/import_template/szablon_importu.xlsx
+++ b/src/main/webapp/src/assets/files/import_template/szablon_importu.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\72846\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -26,74 +22,77 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>imię</t>
-  </si>
-  <si>
-    <t>drugie imię</t>
-  </si>
-  <si>
-    <t>nazwisko</t>
-  </si>
-  <si>
-    <t>pleć</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Pesel</t>
-  </si>
-  <si>
-    <t>nr paszportu</t>
-  </si>
-  <si>
-    <t>kraj wydania</t>
-  </si>
-  <si>
-    <t>data ważności</t>
-  </si>
-  <si>
-    <t>data urodzenia</t>
-  </si>
-  <si>
-    <t>miejsce urodzenia</t>
-  </si>
-  <si>
-    <t>imię ojca</t>
-  </si>
-  <si>
-    <t>imię matki</t>
-  </si>
-  <si>
-    <t>Kod obywatelstwa ISO 3166-1 alfa-2</t>
-  </si>
-  <si>
-    <t>kod kraju ISO 3166-1 alfa-2</t>
-  </si>
-  <si>
-    <t>Miasto</t>
-  </si>
-  <si>
-    <t>ulica</t>
-  </si>
-  <si>
-    <t>numer ulicy</t>
-  </si>
-  <si>
-    <t>numer mieszkania</t>
-  </si>
-  <si>
-    <t>nr telefonu</t>
-  </si>
-  <si>
-    <t>kod pocztowy</t>
+    <t xml:space="preserve">imię</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drugie imię</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nazwisko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">płeć</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nr paszportu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kraj wydania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data ważności</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data urodzenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miejsce urodzenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imię ojca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imię matki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kod obywatelstwa ISO 3166-1 alfa-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kod kraju ISO 3166-1 alfa-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miasto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ulica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numer ulicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numer mieszkania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kod pocztowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nr telefonu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,8 +101,25 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +131,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -123,388 +139,155 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
-  <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" customWidth="1"/>
-    <col min="16" max="16" width="40.5703125" customWidth="1"/>
-    <col min="17" max="17" width="30.42578125" customWidth="1"/>
-    <col min="19" max="19" width="20.140625" customWidth="1"/>
-    <col min="20" max="20" width="45.28515625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="45.29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -523,7 +306,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -542,7 +325,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -561,7 +344,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -580,7 +363,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -599,7 +382,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -618,7 +401,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -637,7 +420,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -656,7 +439,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -675,7 +458,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -694,7 +477,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -713,7 +496,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -732,7 +515,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -751,7 +534,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -770,7 +553,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -789,7 +572,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -808,7 +591,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -827,7 +610,7 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -846,7 +629,7 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -865,7 +648,7 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -884,7 +667,7 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -903,7 +686,7 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -922,7 +705,7 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -941,7 +724,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -960,7 +743,7 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -979,7 +762,7 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -998,7 +781,7 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1017,7 +800,7 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1036,7 +819,7 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1055,7 +838,7 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1074,7 +857,7 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1093,7 +876,7 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1112,7 +895,7 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1131,7 +914,7 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1150,7 +933,7 @@
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1169,7 +952,7 @@
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1188,7 +971,7 @@
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1207,7 +990,7 @@
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1226,7 +1009,7 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1245,7 +1028,7 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1264,7 +1047,7 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1283,7 +1066,7 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1302,7 +1085,7 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1321,7 +1104,7 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1340,7 +1123,7 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1359,7 +1142,7 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1378,7 +1161,7 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1397,7 +1180,7 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1416,7 +1199,7 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -1435,7 +1218,7 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -1454,7 +1237,7 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -1473,7 +1256,7 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -1492,7 +1275,7 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -1511,7 +1294,7 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -1530,7 +1313,7 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -1549,7 +1332,7 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -1568,7 +1351,7 @@
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1587,7 +1370,7 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1606,7 +1389,7 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -1625,7 +1408,7 @@
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -1644,7 +1427,7 @@
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -1663,7 +1446,7 @@
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -1682,7 +1465,7 @@
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1701,7 +1484,7 @@
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1720,7 +1503,7 @@
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -1739,7 +1522,7 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1758,7 +1541,7 @@
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -1777,7 +1560,7 @@
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1796,7 +1579,7 @@
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1815,7 +1598,7 @@
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1834,7 +1617,7 @@
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -1853,7 +1636,7 @@
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1872,7 +1655,7 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1891,7 +1674,7 @@
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -1910,7 +1693,7 @@
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -1929,7 +1712,7 @@
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -1948,7 +1731,7 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -1967,7 +1750,7 @@
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -1986,7 +1769,7 @@
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2006,9 +1789,10 @@
       <c r="U80" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>

</xml_diff>